<commit_message>
Update TTC STation in LIne
Update TTC STation in LIne
</commit_message>
<xml_diff>
--- a/ttc-2019-delays/data/TTC Stations In order by line.xlsx
+++ b/ttc-2019-delays/data/TTC Stations In order by line.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenni\Documents\GitHub\TTC_Subway_Delay_Dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documents\GitHub\Project1\TTC_Subway_Delay_Dashboard\ttc-2019-delays\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_A866DC12DB8DFCEC3BCB88CB87F75817D9435D98" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CFC4ED08-6200-476D-BA3E-AFD3FF30B155}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$81</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="91">
   <si>
     <t>station</t>
   </si>
@@ -80,9 +92,6 @@
     <t>ST CLAIR STATION</t>
   </si>
   <si>
-    <t>BLOOR STATION</t>
-  </si>
-  <si>
     <t>WELLESLEY STATION</t>
   </si>
   <si>
@@ -116,9 +125,6 @@
     <t>LAWRENCE STATION</t>
   </si>
   <si>
-    <t>SHEPPARD STATION</t>
-  </si>
-  <si>
     <t>FINCH STATION</t>
   </si>
   <si>
@@ -140,9 +146,6 @@
     <t>ST PATRICK STATION</t>
   </si>
   <si>
-    <t>QUEENS PARK STATION</t>
-  </si>
-  <si>
     <t>MUSEUM STATION</t>
   </si>
   <si>
@@ -218,9 +221,6 @@
     <t>BAY STATION</t>
   </si>
   <si>
-    <t>BLOOR DANFORTH SUBWAY</t>
-  </si>
-  <si>
     <t>SHERBOURNE STATION</t>
   </si>
   <si>
@@ -278,9 +278,6 @@
     <t>MCCOWAN STATION</t>
   </si>
   <si>
-    <t>SHEPPARD-YONGE STATION</t>
-  </si>
-  <si>
     <t>BAYVIEW STATION</t>
   </si>
   <si>
@@ -291,16 +288,37 @@
   </si>
   <si>
     <t>DON MILLS STATION</t>
+  </si>
+  <si>
+    <t>QUEEN'S PARK STATION</t>
+  </si>
+  <si>
+    <t>SHEPPARD-YONGE SHP STATION</t>
+  </si>
+  <si>
+    <t>SHEPPARD-YONGE YUS STATION</t>
+  </si>
+  <si>
+    <t>YONGE BLOOR BD STATION</t>
+  </si>
+  <si>
+    <t>YONGE BLOOR YUS STATION</t>
+  </si>
+  <si>
+    <t>avg_delay_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">num_delays </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +335,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1D1C1D"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -425,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -433,8 +457,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -458,8 +482,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -469,9 +493,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,21 +776,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.08984375" customWidth="1"/>
+    <col min="1" max="1" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -778,8 +803,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -790,10 +821,16 @@
         <v>-79.313900000000004</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E2">
+        <v>4.92</v>
+      </c>
+      <c r="F2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -804,10 +841,16 @@
         <v>-79.313900000000004</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E3">
+        <v>6.13</v>
+      </c>
+      <c r="F3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -818,12 +861,18 @@
         <v>-79.303399999999996</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E4">
+        <v>14.05</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1">
         <v>43.744900000000001</v>
@@ -832,10 +881,16 @@
         <v>-79.406700000000001</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E5">
+        <v>5.29</v>
+      </c>
+      <c r="F5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -846,10 +901,16 @@
         <v>-79.2453</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E6">
+        <v>6.58</v>
+      </c>
+      <c r="F6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -860,10 +921,16 @@
         <v>-79.201599999999999</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E7">
+        <v>7.03</v>
+      </c>
+      <c r="F7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -874,10 +941,16 @@
         <v>-79.4619</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>5.93</v>
+      </c>
+      <c r="F8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -888,10 +961,16 @@
         <v>-79.450900000000004</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E9">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="F9">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -902,24 +981,36 @@
         <v>-79.448800000000006</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E10">
+        <v>6.63</v>
+      </c>
+      <c r="F10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2">
         <v>-79.263900000000007</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11">
+        <v>6.02</v>
+      </c>
+      <c r="F11">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -930,10 +1021,16 @@
         <v>-79.262699999999995</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E12">
+        <v>11.55</v>
+      </c>
+      <c r="F12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -944,10 +1041,16 @@
         <v>-79.260900000000007</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E13">
+        <v>7.76</v>
+      </c>
+      <c r="F13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -958,12 +1061,18 @@
         <v>-79.233500000000006</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E14">
+        <v>5.91</v>
+      </c>
+      <c r="F14">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>43.402900000000002</v>
@@ -972,12 +1081,18 @@
         <v>-79.242500000000007</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E15">
+        <v>5.75</v>
+      </c>
+      <c r="F15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3">
         <v>43.400199999999998</v>
@@ -986,12 +1101,18 @@
         <v>-79.241399999999999</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E16">
+        <v>8.11</v>
+      </c>
+      <c r="F16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3">
         <v>43.400500000000001</v>
@@ -1000,12 +1121,18 @@
         <v>-79.235900000000001</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E17">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="F17">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1">
         <v>43.400199999999998</v>
@@ -1014,12 +1141,18 @@
         <v>-79.233699999999999</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E18">
+        <v>5.57</v>
+      </c>
+      <c r="F18">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B19" s="1">
         <v>43.393599999999999</v>
@@ -1028,12 +1161,18 @@
         <v>-79.232600000000005</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <v>6.57</v>
+      </c>
+      <c r="F19">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1">
         <v>43.3917</v>
@@ -1042,12 +1181,18 @@
         <v>-79.231800000000007</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E20">
+        <v>5.35</v>
+      </c>
+      <c r="F20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1">
         <v>43.390300000000003</v>
@@ -1056,12 +1201,18 @@
         <v>-79.231200000000001</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E21">
+        <v>8.74</v>
+      </c>
+      <c r="F21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1">
         <v>43.6477</v>
@@ -1070,12 +1221,18 @@
         <v>-79.384799999999998</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E22">
+        <v>6.21</v>
+      </c>
+      <c r="F22">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
         <v>43.645299999999999</v>
@@ -1084,12 +1241,18 @@
         <v>-79.380600000000001</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E23">
+        <v>6.22</v>
+      </c>
+      <c r="F23">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1">
         <v>43.3857</v>
@@ -1098,12 +1261,18 @@
         <v>-79.224000000000004</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24">
+        <v>6.74</v>
+      </c>
+      <c r="F24">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1">
         <v>43.390900000000002</v>
@@ -1112,12 +1281,18 @@
         <v>-79.224500000000006</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E25">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="F25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1">
         <v>43.656300000000002</v>
@@ -1126,12 +1301,18 @@
         <v>-79.380499999999998</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E26">
+        <v>7.36</v>
+      </c>
+      <c r="F26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="1">
         <v>43.394100000000002</v>
@@ -1140,12 +1321,18 @@
         <v>-79.225899999999996</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E27">
+        <v>9.86</v>
+      </c>
+      <c r="F27">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="12">
         <v>43.395499999999998</v>
@@ -1154,12 +1341,18 @@
         <v>-79.230199999999996</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E28">
+        <v>7.02</v>
+      </c>
+      <c r="F28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="B29" s="3">
         <v>43.401600000000002</v>
@@ -1168,12 +1361,18 @@
         <v>-79.230900000000005</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E29">
+        <v>6.4</v>
+      </c>
+      <c r="F29">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B30" s="1">
         <v>43.403700000000001</v>
@@ -1182,12 +1381,18 @@
         <v>-79.231999999999999</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E30">
+        <v>6.53</v>
+      </c>
+      <c r="F30">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1">
         <v>43.4056</v>
@@ -1196,10 +1401,16 @@
         <v>-79.232699999999994</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E31">
+        <v>9.26</v>
+      </c>
+      <c r="F31">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1210,12 +1421,18 @@
         <v>-79.233500000000006</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E32">
+        <v>5.96</v>
+      </c>
+      <c r="F32">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1">
         <v>43.415199999999999</v>
@@ -1224,12 +1441,18 @@
         <v>-79.234999999999999</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E33">
+        <v>6.5</v>
+      </c>
+      <c r="F33">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34" s="1">
         <v>43.4221</v>
@@ -1238,12 +1461,18 @@
         <v>-79.235399999999998</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E34">
+        <v>6.2</v>
+      </c>
+      <c r="F34">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1">
         <v>43.433</v>
@@ -1252,10 +1481,16 @@
         <v>-79.248000000000005</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E35">
+        <v>8.86</v>
+      </c>
+      <c r="F35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -1266,12 +1501,18 @@
         <v>-79.406700000000001</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E36">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="F36">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B37" s="1">
         <v>43.762</v>
@@ -1280,12 +1521,18 @@
         <v>-79.411900000000003</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E37">
+        <v>5.48</v>
+      </c>
+      <c r="F37">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B38" s="1">
         <v>43.761499999999998</v>
@@ -1294,12 +1541,18 @@
         <v>-79.411100000000005</v>
       </c>
       <c r="D38" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38">
+        <v>7.33</v>
+      </c>
+      <c r="F38">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1">
         <v>43.781399999999998</v>
@@ -1308,12 +1561,18 @@
         <v>-79.415000000000006</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+      <c r="E39">
+        <v>4.01</v>
+      </c>
+      <c r="F39">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B40" s="3">
         <v>43.381399999999999</v>
@@ -1322,12 +1581,18 @@
         <v>-79.320999999999998</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E40">
+        <v>5.15</v>
+      </c>
+      <c r="F40">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B41" s="3">
         <v>43.384300000000003</v>
@@ -1336,12 +1601,18 @@
         <v>-79.312799999999996</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E41">
+        <v>5.56</v>
+      </c>
+      <c r="F41">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B42" s="3">
         <v>43.385300000000001</v>
@@ -1350,12 +1621,18 @@
         <v>-79.304100000000005</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E42">
+        <v>7.12</v>
+      </c>
+      <c r="F42">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B43" s="14">
         <v>43.39</v>
@@ -1364,12 +1641,18 @@
         <v>-79.2941</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E43">
+        <v>10.54</v>
+      </c>
+      <c r="F43">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B44" s="3">
         <v>43.385899999999999</v>
@@ -1378,12 +1661,18 @@
         <v>-79.290199999999999</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E44">
+        <v>7.63</v>
+      </c>
+      <c r="F44">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B45" s="3">
         <v>43.390599999999999</v>
@@ -1392,12 +1681,18 @@
         <v>-79.283299999999997</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E45">
+        <v>9</v>
+      </c>
+      <c r="F45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B46" s="3">
         <v>43.391399999999997</v>
@@ -1406,12 +1701,18 @@
         <v>-79.28</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E46">
+        <v>6.74</v>
+      </c>
+      <c r="F46">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B47" s="3">
         <v>43.392000000000003</v>
@@ -1420,12 +1721,18 @@
         <v>-79.273499999999999</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E47">
+        <v>7.21</v>
+      </c>
+      <c r="F47">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B48" s="3">
         <v>43.392499999999998</v>
@@ -1434,12 +1741,18 @@
         <v>-79.271050000000002</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E48">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F48">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B49" s="3">
         <v>43.393300000000004</v>
@@ -1448,12 +1761,18 @@
         <v>-79.263400000000004</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E49">
+        <v>5.53</v>
+      </c>
+      <c r="F49">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B50" s="3">
         <v>43.393599999999999</v>
@@ -1462,12 +1781,18 @@
         <v>-79.260800000000003</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E50">
+        <v>10.36</v>
+      </c>
+      <c r="F50">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B51" s="3">
         <v>43.394399999999997</v>
@@ -1476,12 +1801,18 @@
         <v>-79.253600000000006</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E51">
+        <v>7.32</v>
+      </c>
+      <c r="F51">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B52" s="3">
         <v>43.395099999999999</v>
@@ -1490,12 +1821,18 @@
         <v>-79.250600000000006</v>
       </c>
       <c r="D52" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52">
+        <v>5.34</v>
+      </c>
+      <c r="F52">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B53" s="3">
         <v>43.395800000000001</v>
@@ -1504,12 +1841,18 @@
         <v>-79.244</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E53">
+        <v>6.23</v>
+      </c>
+      <c r="F53">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B54" s="1">
         <v>43.400199999999998</v>
@@ -1518,12 +1861,18 @@
         <v>-79.241399999999999</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E54">
+        <v>10.52</v>
+      </c>
+      <c r="F54">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B55" s="1">
         <v>43.668300000000002</v>
@@ -1532,12 +1881,18 @@
         <v>-79.399900000000002</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E55">
+        <v>8.42</v>
+      </c>
+      <c r="F55">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B56" s="3">
         <v>43.401299999999999</v>
@@ -1546,12 +1901,18 @@
         <v>-79.232399999999998</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
-        <v>64</v>
+        <v>41</v>
+      </c>
+      <c r="E56">
+        <v>5.8</v>
+      </c>
+      <c r="F56">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>87</v>
       </c>
       <c r="B57" s="1">
         <v>43.6706</v>
@@ -1560,12 +1921,18 @@
         <v>-79.386499999999998</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E57">
+        <v>5.94</v>
+      </c>
+      <c r="F57">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B58" s="3">
         <v>43.402000000000001</v>
@@ -1574,12 +1941,18 @@
         <v>-79.223500000000001</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E58">
+        <v>5.9</v>
+      </c>
+      <c r="F58">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B59" s="3">
         <v>43.402500000000003</v>
@@ -1588,12 +1961,18 @@
         <v>-79.220799999999997</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E59">
+        <v>8.92</v>
+      </c>
+      <c r="F59">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B60" s="3">
         <v>43.403700000000001</v>
@@ -1602,12 +1981,18 @@
         <v>-79.212999999999994</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E60">
+        <v>6.11</v>
+      </c>
+      <c r="F60">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B61" s="3">
         <v>43.404200000000003</v>
@@ -1616,12 +2001,18 @@
         <v>-79.210899999999995</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E61">
+        <v>7.23</v>
+      </c>
+      <c r="F61">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B62" s="3">
         <v>43.404800000000002</v>
@@ -1630,12 +2021,18 @@
         <v>-79.2042</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E62">
+        <v>5.41</v>
+      </c>
+      <c r="F62">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B63" s="17">
         <v>43.680999999999997</v>
@@ -1644,12 +2041,18 @@
         <v>-79.337800000000001</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+      <c r="E63">
+        <v>5.73</v>
+      </c>
+      <c r="F63">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B64" s="19">
         <v>43.405700000000003</v>
@@ -1658,12 +2061,18 @@
         <v>-79.194900000000004</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E64">
+        <v>5.73</v>
+      </c>
+      <c r="F64">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B65" s="3">
         <v>43.410299999999999</v>
@@ -1672,12 +2081,18 @@
         <v>-79.192300000000003</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E65">
+        <v>4.71</v>
+      </c>
+      <c r="F65">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B66" s="3">
         <v>43.411099999999998</v>
@@ -1686,12 +2101,18 @@
         <v>-79.184600000000003</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E66">
+        <v>8.86</v>
+      </c>
+      <c r="F66">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B67" s="3">
         <v>43.412050000000001</v>
@@ -1700,12 +2121,18 @@
         <v>-79.180599999999998</v>
       </c>
       <c r="D67" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E67">
+        <v>5.61</v>
+      </c>
+      <c r="F67">
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B68" s="3">
         <v>43.414200000000001</v>
@@ -1714,12 +2141,18 @@
         <v>-79.171899999999994</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E68">
+        <v>9.52</v>
+      </c>
+      <c r="F68">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B69" s="3">
         <v>43.424100000000003</v>
@@ -1728,12 +2161,18 @@
         <v>-79.164699999999996</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E69">
+        <v>6.69</v>
+      </c>
+      <c r="F69">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B70" s="3">
         <v>43.435699999999997</v>
@@ -1742,12 +2181,18 @@
         <v>-79.154899999999998</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="E70">
+        <v>4.57</v>
+      </c>
+      <c r="F70">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B71" s="3">
         <v>43.732500000000002</v>
@@ -1756,12 +2201,18 @@
         <v>-79.263599999999997</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="E71">
+        <v>14.65</v>
+      </c>
+      <c r="F71">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B72" s="20">
         <v>43.450099999999999</v>
@@ -1770,12 +2221,18 @@
         <v>-79.161299999999997</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="E72">
+        <v>15.66</v>
+      </c>
+      <c r="F72">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B73" s="20">
         <v>43.460099999999997</v>
@@ -1784,12 +2241,18 @@
         <v>-79.163499999999999</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="E73">
+        <v>11.62</v>
+      </c>
+      <c r="F73">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B74" s="3">
         <v>43.461350000000003</v>
@@ -1798,12 +2261,18 @@
         <v>-79.161900000000003</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="E74">
+        <v>4.95</v>
+      </c>
+      <c r="F74">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B75" s="20">
         <v>43.462800000000001</v>
@@ -1812,12 +2281,18 @@
         <v>-79.152799999999999</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="E75">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="F75">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B76" s="20">
         <v>43.462899999999998</v>
@@ -1826,12 +2301,18 @@
         <v>-79.150599999999997</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A77" s="5" t="s">
-        <v>84</v>
+        <v>42</v>
+      </c>
+      <c r="E76">
+        <v>8.34</v>
+      </c>
+      <c r="F76">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>85</v>
       </c>
       <c r="B77" s="1">
         <v>43.762</v>
@@ -1840,12 +2321,18 @@
         <v>-79.411900000000003</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="E77">
+        <v>5.42</v>
+      </c>
+      <c r="F77">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B78" s="20">
         <v>43.460099999999997</v>
@@ -1854,12 +2341,18 @@
         <v>-79.231200000000001</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="E78">
+        <v>13.3</v>
+      </c>
+      <c r="F78">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B79" s="20">
         <v>43.460900000000002</v>
@@ -1868,12 +2361,18 @@
         <v>-79.223500000000001</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="E79">
+        <v>5.45</v>
+      </c>
+      <c r="F79">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B80" s="20">
         <v>43.4617</v>
@@ -1882,12 +2381,18 @@
         <v>-79.215500000000006</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="E80">
+        <v>6.81</v>
+      </c>
+      <c r="F80">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B81" s="20">
         <v>43.775700000000001</v>
@@ -1896,7 +2401,13 @@
         <v>-79.345399999999998</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="E81">
+        <v>5.49</v>
+      </c>
+      <c r="F81">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>